<commit_message>
debug: comma in data affect the csv file
</commit_message>
<xml_diff>
--- a/Hot100_20170408.xlsx
+++ b/Hot100_20170408.xlsx
@@ -17,7 +17,7 @@
     <sheet name="工作表3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="data" localSheetId="0">工作表1!$A$1:$G$101</definedName>
+    <definedName name="data" localSheetId="0">工作表1!$A$1:$F$101</definedName>
   </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -519,6 +519,9 @@
     <t xml:space="preserve"> No Frauds </t>
   </si>
   <si>
+    <t xml:space="preserve"> Nicki Minaj  Drake &amp; Lil Wayne</t>
+  </si>
+  <si>
     <t xml:space="preserve"> Selfish </t>
   </si>
   <si>
@@ -598,10 +601,6 @@
   </si>
   <si>
     <t xml:space="preserve"> The Weeknd</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Nicki Minaj,  Drake &amp; Lil Wayne</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -930,7 +929,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
       <selection activeCell="F85" sqref="F85"/>
     </sheetView>
   </sheetViews>
@@ -942,7 +941,6 @@
     <col min="4" max="4" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="45.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -2642,7 +2640,7 @@
         <v>2</v>
       </c>
       <c r="F85" t="s">
-        <v>183</v>
+        <v>156</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.2">
@@ -2650,7 +2648,7 @@
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C86">
         <v>59</v>
@@ -2662,7 +2660,7 @@
         <v>4</v>
       </c>
       <c r="F86" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.2">
@@ -2670,7 +2668,7 @@
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C87">
         <v>67</v>
@@ -2682,7 +2680,7 @@
         <v>6</v>
       </c>
       <c r="F87" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.2">
@@ -2690,7 +2688,7 @@
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C88">
         <v>80</v>
@@ -2702,7 +2700,7 @@
         <v>9</v>
       </c>
       <c r="F88" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.2">
@@ -2710,7 +2708,7 @@
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C89" t="s">
         <v>21</v>
@@ -2722,7 +2720,7 @@
         <v>1</v>
       </c>
       <c r="F89" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.2">
@@ -2730,7 +2728,7 @@
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C90">
         <v>63</v>
@@ -2750,7 +2748,7 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C91">
         <v>75</v>
@@ -2762,7 +2760,7 @@
         <v>12</v>
       </c>
       <c r="F91" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.2">
@@ -2770,7 +2768,7 @@
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C92">
         <v>79</v>
@@ -2782,7 +2780,7 @@
         <v>4</v>
       </c>
       <c r="F92" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.2">
@@ -2790,7 +2788,7 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C93">
         <v>81</v>
@@ -2802,7 +2800,7 @@
         <v>4</v>
       </c>
       <c r="F93" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.2">
@@ -2810,7 +2808,7 @@
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C94">
         <v>84</v>
@@ -2822,7 +2820,7 @@
         <v>12</v>
       </c>
       <c r="F94" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.2">
@@ -2830,7 +2828,7 @@
         <v>94</v>
       </c>
       <c r="B95" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C95">
         <v>60</v>
@@ -2850,7 +2848,7 @@
         <v>95</v>
       </c>
       <c r="B96" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C96">
         <v>74</v>
@@ -2870,7 +2868,7 @@
         <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C97">
         <v>83</v>
@@ -2882,7 +2880,7 @@
         <v>15</v>
       </c>
       <c r="F97" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.2">
@@ -2890,7 +2888,7 @@
         <v>97</v>
       </c>
       <c r="B98" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C98" t="s">
         <v>21</v>
@@ -2902,7 +2900,7 @@
         <v>1</v>
       </c>
       <c r="F98" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.2">
@@ -2910,7 +2908,7 @@
         <v>98</v>
       </c>
       <c r="B99" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C99" t="s">
         <v>21</v>
@@ -2922,7 +2920,7 @@
         <v>1</v>
       </c>
       <c r="F99" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.2">
@@ -2930,7 +2928,7 @@
         <v>99</v>
       </c>
       <c r="B100" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C100">
         <v>77</v>
@@ -2942,7 +2940,7 @@
         <v>18</v>
       </c>
       <c r="F100" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>